<commit_message>
Added descriptions to CLR
</commit_message>
<xml_diff>
--- a/ideas/CLR/CLR_standard_input_ideas.xlsx
+++ b/ideas/CLR/CLR_standard_input_ideas.xlsx
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="640">
   <si>
     <t>text</t>
   </si>
@@ -2075,6 +2075,12 @@
   </si>
   <si>
     <t>2016-12-31</t>
+  </si>
+  <si>
+    <t>IDEAS aims to encourage interdisciplinary artists and musicians, as well as engineers and scientists to take advantage of the Qualcomm Institute’s advanced audio-visual facilities, services and personnel in staging performances and presentations of new or existing works and research. This collection contains video, still images, audio, and text, documenting past performances and presentations from the ongoing series.</t>
+  </si>
+  <si>
+    <t>This collection contains video, still images, audio, and text, documenting past IDEAS performances and presentations from the ongoing series.</t>
   </si>
 </sst>
 </file>
@@ -3119,8 +3125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3194,7 +3200,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="165" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>631</v>
       </c>
@@ -3221,6 +3227,12 @@
       </c>
       <c r="K2" s="3" t="s">
         <v>637</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>638</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added topics and tried to finish up CLR
</commit_message>
<xml_diff>
--- a/ideas/CLR/CLR_standard_input_ideas.xlsx
+++ b/ideas/CLR/CLR_standard_input_ideas.xlsx
@@ -40,7 +40,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -107,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -142,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="643">
   <si>
     <t>text</t>
   </si>
@@ -2081,6 +2081,15 @@
   </si>
   <si>
     <t>This collection contains video, still images, audio, and text, documenting past IDEAS performances and presentations from the ongoing series.</t>
+  </si>
+  <si>
+    <t>Computer music | Performing arts | Multimedia installations (Art) | Installations (Art) | Performance art | Opera | Video games | Drama</t>
+  </si>
+  <si>
+    <t>Interactive multimedia</t>
+  </si>
+  <si>
+    <t>IDEAS Web site via Calit2 @ http://ideas.calit2.net/</t>
   </si>
 </sst>
 </file>
@@ -3123,10 +3132,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3136,18 +3145,17 @@
     <col min="4" max="4" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" style="3" customWidth="1"/>
     <col min="6" max="6" width="51.5703125" style="3" customWidth="1"/>
-    <col min="7" max="8" width="45.140625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="45.5703125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="58.85546875" style="3" customWidth="1"/>
-    <col min="13" max="14" width="39.140625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="42.85546875" style="3" customWidth="1"/>
-    <col min="16" max="16" width="44.5703125" style="3" customWidth="1"/>
-    <col min="17" max="17" width="84.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="45.140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="45.5703125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="58.85546875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="39.140625" style="3" customWidth="1"/>
+    <col min="13" max="14" width="42.85546875" style="3" customWidth="1"/>
+    <col min="15" max="15" width="84.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>337</v>
       </c>
@@ -3167,40 +3175,34 @@
         <v>1</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>515</v>
+        <v>300</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>300</v>
+        <v>486</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>486</v>
+        <v>5</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="K1" s="17" t="s">
         <v>620</v>
       </c>
+      <c r="L1" s="16" t="s">
+        <v>3</v>
+      </c>
       <c r="M1" s="16" t="s">
-        <v>3</v>
+        <v>459</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>519</v>
+        <v>450</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>520</v>
-      </c>
-      <c r="P1" s="16" t="s">
-        <v>521</v>
-      </c>
-      <c r="Q1" s="16" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="165" x14ac:dyDescent="0.25">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>631</v>
       </c>
@@ -3216,23 +3218,32 @@
       <c r="F2" s="3" t="s">
         <v>633</v>
       </c>
+      <c r="G2" s="3" t="s">
+        <v>634</v>
+      </c>
       <c r="H2" s="3" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>638</v>
+        <v>640</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>642</v>
       </c>
     </row>
   </sheetData>
@@ -3244,7 +3255,7 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="11">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
           <x14:formula1>
             <xm:f>'CV values'!$C$2:$C$15</xm:f>
@@ -3267,49 +3278,31 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$C$1:$C$185</xm:f>
           </x14:formula1>
-          <xm:sqref>H1</xm:sqref>
+          <xm:sqref>G1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$D$1:$D$6</xm:f>
           </x14:formula1>
-          <xm:sqref>I1</xm:sqref>
+          <xm:sqref>H1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$G$1:$G$17</xm:f>
           </x14:formula1>
-          <xm:sqref>O1</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
-          <x14:formula1>
-            <xm:f>'Select-a-header values'!$H$1:$H$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>P1</xm:sqref>
+          <xm:sqref>M1:N1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$I$1:$I$12</xm:f>
           </x14:formula1>
-          <xm:sqref>Q1</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
-          <x14:formula1>
-            <xm:f>'Select-a-header values'!$B$1:$B$233</xm:f>
-          </x14:formula1>
-          <xm:sqref>G1</xm:sqref>
+          <xm:sqref>O1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$E$1:$E$34</xm:f>
           </x14:formula1>
-          <xm:sqref>M1</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
-          <x14:formula1>
-            <xm:f>'Select-a-header values'!$F$1:$F$21</xm:f>
-          </x14:formula1>
-          <xm:sqref>N1</xm:sqref>
+          <xm:sqref>L1</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Updated CLR to reflect QA issues
</commit_message>
<xml_diff>
--- a/ideas/CLR/CLR_standard_input_ideas.xlsx
+++ b/ideas/CLR/CLR_standard_input_ideas.xlsx
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="642">
   <si>
     <t>text</t>
   </si>
@@ -2083,13 +2083,10 @@
     <t>This collection contains video, still images, audio, and text, documenting past IDEAS performances and presentations from the ongoing series.</t>
   </si>
   <si>
-    <t>Computer music | Performing arts | Multimedia installations (Art) | Installations (Art) | Performance art | Opera | Video games | Drama</t>
-  </si>
-  <si>
-    <t>Interactive multimedia</t>
-  </si>
-  <si>
     <t>IDEAS Web site via Calit2 @ http://ideas.calit2.net/</t>
+  </si>
+  <si>
+    <t>Computer music | Multimedia installations (Art) | Installations (Art) | Performance art | Opera | Video games | Drama</t>
   </si>
 </sst>
 </file>
@@ -3132,10 +3129,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3151,11 +3148,11 @@
     <col min="10" max="10" width="15.140625" style="3" customWidth="1"/>
     <col min="11" max="11" width="58.85546875" style="3" customWidth="1"/>
     <col min="12" max="12" width="39.140625" style="3" customWidth="1"/>
-    <col min="13" max="14" width="42.85546875" style="3" customWidth="1"/>
-    <col min="15" max="15" width="84.28515625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="42.85546875" style="3" customWidth="1"/>
+    <col min="14" max="14" width="84.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>337</v>
       </c>
@@ -3196,13 +3193,10 @@
         <v>459</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>450</v>
-      </c>
-      <c r="O1" s="16" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="180" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="165" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>631</v>
       </c>
@@ -3237,13 +3231,10 @@
         <v>638</v>
       </c>
       <c r="M2" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>640</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>641</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>642</v>
       </c>
     </row>
   </sheetData>
@@ -3290,13 +3281,13 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$G$1:$G$17</xm:f>
           </x14:formula1>
-          <xm:sqref>M1:N1</xm:sqref>
+          <xm:sqref>M1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$I$1:$I$12</xm:f>
           </x14:formula1>
-          <xm:sqref>O1</xm:sqref>
+          <xm:sqref>N1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>

</xml_diff>

<commit_message>
Updated CLR for final production ingest
</commit_message>
<xml_diff>
--- a/ideas/CLR/CLR_standard_input_ideas.xlsx
+++ b/ideas/CLR/CLR_standard_input_ideas.xlsx
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="643">
   <si>
     <t>text</t>
   </si>
@@ -2087,6 +2087,9 @@
   </si>
   <si>
     <t>Computer music | Multimedia installations (Art) | Installations (Art) | Performance art | Opera | Video games | Drama</t>
+  </si>
+  <si>
+    <t>IDEAS_crowd_cave.jpg</t>
   </si>
 </sst>
 </file>
@@ -3131,8 +3134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3202,6 +3205,9 @@
       </c>
       <c r="B2" s="3" t="s">
         <v>632</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>642</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>340</v>

</xml_diff>